<commit_message>
Update hentai level logic, add brown color, fix witness card feedback
</commit_message>
<xml_diff>
--- a/変態は踊るWebゲーム開発指示書.xlsx
+++ b/変態は踊るWebゲーム開発指示書.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbfa402375cd2dd8/Desktop/game/変態は踊る/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="548" documentId="13_ncr:1_{F1ACA8C2-00E5-42E4-8CE6-1E272D4FAC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DAEC812-1A50-42D0-8148-3B3B1AE87667}"/>
+  <xr:revisionPtr revIDLastSave="555" documentId="13_ncr:1_{F1ACA8C2-00E5-42E4-8CE6-1E272D4FAC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FB0777A-AD57-4646-9B29-20917738D689}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="877">
   <si>
     <t>あなたは熟練したWebゲーム開発者です。</t>
   </si>
@@ -3542,6 +3542,21 @@
     <rPh sb="6" eb="7">
       <t>ナカ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>浮気中⇒</t>
+    <rPh sb="0" eb="3">
+      <t>ウワキチュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ホモ⇒</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>チョコボール・</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3801,6 +3816,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3810,7 +3843,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3828,31 +3861,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -17474,16 +17489,17 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976779D7-B276-4C4F-9A83-5B750AA20676}">
-  <dimension ref="A2:F38"/>
+  <dimension ref="A2:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17923,6 +17939,9 @@
       <c r="C35" t="s">
         <v>859</v>
       </c>
+      <c r="E35" t="s">
+        <v>876</v>
+      </c>
     </row>
     <row r="36" spans="3:6">
       <c r="C36" t="s">
@@ -17937,6 +17956,16 @@
     <row r="38" spans="3:6">
       <c r="C38" t="s">
         <v>873</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6">
+      <c r="C40" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6">
+      <c r="C41" t="s">
+        <v>875</v>
       </c>
     </row>
   </sheetData>
@@ -18885,196 +18914,196 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.5">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="23" t="s">
         <v>601</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="17" t="s">
         <v>411</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="33" t="s">
         <v>412</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="29" t="s">
         <v>514</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="23" t="s">
         <v>517</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="20">
         <v>99</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="32" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="18"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="18"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:8" ht="43.5" thickBot="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="19"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:8" ht="42.75">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="23" t="s">
         <v>598</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="17" t="s">
         <v>665</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="34" t="s">
         <v>435</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="29" t="s">
         <v>520</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="20" t="s">
         <v>521</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="20">
         <v>20</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="21" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="18"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="27"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" ht="19.5" thickBot="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="28"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="19"/>
       <c r="F8" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:8" ht="28.5">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="29" t="s">
         <v>514</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="20" t="s">
         <v>523</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="20">
         <v>30</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="21" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="18"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="27"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" ht="44.25" thickBot="1">
-      <c r="A11" s="19"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="28"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
     </row>
     <row r="12" spans="1:8" ht="28.5">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="17" t="s">
         <v>602</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="33" t="s">
         <v>437</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="29" t="s">
         <v>514</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="20" t="s">
         <v>523</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="20">
         <v>40</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="21" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="18"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="27"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="18"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" ht="29.25" thickBot="1">
-      <c r="A14" s="19"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="28"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:8" ht="83.25" customHeight="1" thickBot="1">
       <c r="A15" s="1" t="s">
@@ -19103,288 +19132,288 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.5">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="29" t="s">
         <v>528</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="20" t="s">
         <v>523</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="20">
         <v>60</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="H16" s="21" t="s">
         <v>549</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="18"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="27"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" ht="29.25" thickBot="1">
-      <c r="A18" s="19"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="28"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8" ht="28.5">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="29" t="s">
         <v>528</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="20" t="s">
         <v>523</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="20">
         <v>65</v>
       </c>
-      <c r="H19" s="32" t="s">
+      <c r="H19" s="21" t="s">
         <v>550</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="18"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="27"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" ht="43.5" thickBot="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="28"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:8" ht="28.5">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="17" t="s">
         <v>434</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="33" t="s">
         <v>448</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="29" t="s">
         <v>520</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="20" t="s">
         <v>523</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="20">
         <v>70</v>
       </c>
-      <c r="H22" s="32" t="s">
+      <c r="H22" s="21" t="s">
         <v>667</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="18"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="27"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="18"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
     </row>
     <row r="24" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A24" s="18"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="27"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="18"/>
       <c r="F24" s="5" t="s">
         <v>540</v>
       </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="18"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="27"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:8" ht="29.25" thickBot="1">
-      <c r="A26" s="19"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="28"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="19"/>
       <c r="F26" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
     </row>
     <row r="27" spans="1:8" ht="28.5">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="29" t="s">
         <v>514</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="E27" s="20" t="s">
         <v>523</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="G27" s="26">
+      <c r="G27" s="20">
         <v>75</v>
       </c>
-      <c r="H27" s="32" t="s">
+      <c r="H27" s="21" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A28" s="18"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="27"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="18"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8" ht="28.5">
-      <c r="A29" s="18"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="27"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="18"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="27"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
     </row>
     <row r="31" spans="1:8" ht="29.25" thickBot="1">
-      <c r="A31" s="19"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="28"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
     </row>
     <row r="32" spans="1:8" ht="28.5">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="29" t="s">
         <v>520</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="20" t="s">
         <v>523</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="G32" s="26">
+      <c r="G32" s="20">
         <v>80</v>
       </c>
-      <c r="H32" s="33" t="s">
+      <c r="H32" s="22" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="18"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="27"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="18"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8" ht="29.25" thickBot="1">
-      <c r="A34" s="19"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="28"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="19"/>
       <c r="F34" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:8" ht="69.75" customHeight="1" thickBot="1">
       <c r="A35" s="1" t="s">
@@ -19412,26 +19441,33 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="H22:H26"/>
-    <mergeCell ref="H27:H31"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="G27:G31"/>
     <mergeCell ref="H3:H5"/>
     <mergeCell ref="H16:H18"/>
     <mergeCell ref="H19:H21"/>
@@ -19448,33 +19484,26 @@
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="C19:C21"/>
     <mergeCell ref="D19:D21"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="E27:E31"/>
-    <mergeCell ref="G27:G31"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="H22:H26"/>
+    <mergeCell ref="H27:H31"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>